<commit_message>
Modularisation mid-point. - Created sector files. - Created init file. - Central CNF file. - Created generic sector file.
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v3.xlsx
+++ b/data/cnf_files/restore_cnf_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6C729F-71B3-D144-8D25-2730DB35D9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE23900-A7C4-3341-A1BA-8E616FC8E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -351,10 +351,10 @@
     <t>enable_max_import_share</t>
   </si>
   <si>
-    <t>max_export_share</t>
+    <t>flow_in_max_share</t>
   </si>
   <si>
-    <t>max_import_share</t>
+    <t>flow_out_max_share</t>
   </si>
 </sst>
 </file>
@@ -3862,9 +3862,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="B315" sqref="B315"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -9663,7 +9669,7 @@
         <v>5</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -9676,7 +9682,7 @@
         <v>5</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -20698,6 +20704,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -28220,7 +28229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E275" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Modularisation complete. Same result as non-modular version :)
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v3.xlsx
+++ b/data/cnf_files/restore_cnf_v3.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE23900-A7C4-3341-A1BA-8E616FC8E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC4B793-5F58-6545-8CA0-D090A18E51CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="36700" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
     <sheet name="convchp" sheetId="2" r:id="rId2"/>
     <sheet name="convelec" sheetId="3" r:id="rId3"/>
     <sheet name="convpassenger" sheetId="4" r:id="rId4"/>
-    <sheet name="convtransdis" sheetId="5" r:id="rId5"/>
+    <sheet name="convenertransp" sheetId="5" r:id="rId5"/>
     <sheet name="dem" sheetId="6" r:id="rId6"/>
     <sheet name="ext" sheetId="7" r:id="rId7"/>
     <sheet name="flow" sheetId="8" r:id="rId8"/>
@@ -243,9 +243,6 @@
     <t>passenger</t>
   </si>
   <si>
-    <t>conv_transdis_elec</t>
-  </si>
-  <si>
     <t>elecdelivered</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>flow_out_max_share</t>
+  </si>
+  <si>
+    <t>conv_enertransp_elec</t>
   </si>
 </sst>
 </file>
@@ -3862,7 +3862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+    <sheetView topLeftCell="A267" workbookViewId="0">
       <selection activeCell="B315" sqref="B315"/>
     </sheetView>
   </sheetViews>
@@ -3886,19 +3886,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4356,7 +4356,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2">
@@ -4383,7 +4383,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2">
@@ -4410,7 +4410,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2">
@@ -4437,7 +4437,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2">
@@ -4464,7 +4464,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2">
@@ -4491,7 +4491,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2">
@@ -4518,7 +4518,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
@@ -4545,7 +4545,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2">
@@ -4572,7 +4572,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
@@ -4599,7 +4599,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -4626,7 +4626,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
@@ -4653,7 +4653,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
@@ -4680,7 +4680,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -4707,7 +4707,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
@@ -4734,7 +4734,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
@@ -4761,7 +4761,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -4788,7 +4788,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -4815,7 +4815,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
@@ -4842,7 +4842,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -4869,7 +4869,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -4896,7 +4896,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -4923,7 +4923,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
@@ -4950,7 +4950,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
@@ -4977,7 +4977,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2">
@@ -5004,7 +5004,7 @@
         <v>8</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
@@ -5031,7 +5031,7 @@
         <v>8</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2">
@@ -5058,7 +5058,7 @@
         <v>8</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2">
@@ -5085,7 +5085,7 @@
         <v>8</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2">
@@ -5112,7 +5112,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2">
@@ -5139,7 +5139,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2">
@@ -5166,7 +5166,7 @@
         <v>8</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2">
@@ -5193,7 +5193,7 @@
         <v>8</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2">
@@ -5220,7 +5220,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2">
@@ -5247,7 +5247,7 @@
         <v>8</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2">
@@ -5274,7 +5274,7 @@
         <v>8</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2">
@@ -5301,7 +5301,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2">
@@ -5328,7 +5328,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2">
@@ -5355,7 +5355,7 @@
         <v>8</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2">
@@ -5382,7 +5382,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
@@ -5409,7 +5409,7 @@
         <v>8</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2">
@@ -5436,7 +5436,7 @@
         <v>8</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2">
@@ -5463,7 +5463,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2">
@@ -5490,7 +5490,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2">
@@ -5517,7 +5517,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2">
@@ -5544,7 +5544,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2">
@@ -5571,7 +5571,7 @@
         <v>8</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2">
@@ -5598,7 +5598,7 @@
         <v>8</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2">
@@ -5625,7 +5625,7 @@
         <v>8</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2">
@@ -5652,7 +5652,7 @@
         <v>8</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2">
@@ -5679,7 +5679,7 @@
         <v>8</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2">
@@ -5706,7 +5706,7 @@
         <v>8</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2">
@@ -5733,7 +5733,7 @@
         <v>8</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2">
@@ -5760,7 +5760,7 @@
         <v>8</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2">
@@ -5787,7 +5787,7 @@
         <v>8</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2">
@@ -5814,7 +5814,7 @@
         <v>8</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2">
@@ -5841,7 +5841,7 @@
         <v>8</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2">
@@ -5868,7 +5868,7 @@
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2">
@@ -5895,7 +5895,7 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2">
@@ -5922,7 +5922,7 @@
         <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2">
@@ -5949,7 +5949,7 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2">
@@ -6876,7 +6876,7 @@
         <v>8</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2">
@@ -6903,7 +6903,7 @@
         <v>8</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2">
@@ -6930,7 +6930,7 @@
         <v>8</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2">
@@ -6957,7 +6957,7 @@
         <v>8</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="2">
@@ -6984,7 +6984,7 @@
         <v>8</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2">
@@ -7011,7 +7011,7 @@
         <v>8</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2">
@@ -7038,7 +7038,7 @@
         <v>8</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2">
@@ -7065,7 +7065,7 @@
         <v>8</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="2">
@@ -7092,7 +7092,7 @@
         <v>8</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="2">
@@ -7119,7 +7119,7 @@
         <v>8</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="2">
@@ -7146,7 +7146,7 @@
         <v>8</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2">
@@ -7173,7 +7173,7 @@
         <v>8</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2">
@@ -7200,7 +7200,7 @@
         <v>8</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2">
@@ -7227,7 +7227,7 @@
         <v>8</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2">
@@ -7254,7 +7254,7 @@
         <v>8</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2">
@@ -7281,7 +7281,7 @@
         <v>8</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="2">
@@ -7308,7 +7308,7 @@
         <v>8</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2">
@@ -7335,7 +7335,7 @@
         <v>8</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2">
@@ -7362,7 +7362,7 @@
         <v>8</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2">
@@ -7389,7 +7389,7 @@
         <v>8</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2">
@@ -7416,7 +7416,7 @@
         <v>8</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2">
@@ -7443,7 +7443,7 @@
         <v>8</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2">
@@ -7470,7 +7470,7 @@
         <v>8</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2">
@@ -7497,7 +7497,7 @@
         <v>8</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2">
@@ -7524,7 +7524,7 @@
         <v>8</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2">
@@ -7551,7 +7551,7 @@
         <v>8</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2">
@@ -7578,7 +7578,7 @@
         <v>8</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="2">
@@ -7605,7 +7605,7 @@
         <v>8</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2">
@@ -7632,7 +7632,7 @@
         <v>8</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="2">
@@ -7659,7 +7659,7 @@
         <v>8</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C181" s="2"/>
       <c r="D181" s="2">
@@ -9036,7 +9036,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2">
@@ -9051,7 +9051,7 @@
         <v>8</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="2">
@@ -9066,7 +9066,7 @@
         <v>8</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="2">
@@ -9081,7 +9081,7 @@
         <v>8</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="2">
@@ -9096,7 +9096,7 @@
         <v>8</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2">
@@ -9111,7 +9111,7 @@
         <v>8</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2">
@@ -9126,7 +9126,7 @@
         <v>8</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="2">
@@ -9141,7 +9141,7 @@
         <v>8</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="2">
@@ -9156,7 +9156,7 @@
         <v>8</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="2">
@@ -9171,7 +9171,7 @@
         <v>8</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="2">
@@ -9186,7 +9186,7 @@
         <v>8</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="2">
@@ -9201,7 +9201,7 @@
         <v>8</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="2">
@@ -9216,7 +9216,7 @@
         <v>8</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2">
@@ -9231,7 +9231,7 @@
         <v>8</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="2">
@@ -9246,7 +9246,7 @@
         <v>8</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="2">
@@ -9261,7 +9261,7 @@
         <v>8</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="2">
@@ -9276,7 +9276,7 @@
         <v>8</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="2">
@@ -9291,7 +9291,7 @@
         <v>8</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="2">
@@ -9306,7 +9306,7 @@
         <v>8</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="2">
@@ -9321,7 +9321,7 @@
         <v>8</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2">
@@ -9336,7 +9336,7 @@
         <v>8</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="2">
@@ -9351,7 +9351,7 @@
         <v>8</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="2">
@@ -9366,7 +9366,7 @@
         <v>8</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2">
@@ -9381,7 +9381,7 @@
         <v>8</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="2">
@@ -9396,7 +9396,7 @@
         <v>8</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2">
@@ -9411,7 +9411,7 @@
         <v>8</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2">
@@ -9426,7 +9426,7 @@
         <v>8</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2">
@@ -9441,7 +9441,7 @@
         <v>8</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="2">
@@ -9456,7 +9456,7 @@
         <v>8</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="2">
@@ -9471,7 +9471,7 @@
         <v>8</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="2">
@@ -9499,7 +9499,7 @@
         <v>33</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -9512,7 +9512,7 @@
         <v>33</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -9537,7 +9537,7 @@
         <v>33</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -9550,7 +9550,7 @@
         <v>33</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -9669,7 +9669,7 @@
         <v>5</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -9682,7 +9682,7 @@
         <v>5</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -9789,9 +9789,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
@@ -9807,7 +9812,7 @@
         <v>67</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>54</v>
@@ -9962,7 +9967,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -9970,7 +9975,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -9978,7 +9983,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -9986,7 +9991,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -9994,17 +9999,17 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -10012,12 +10017,12 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -10029,9 +10034,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
@@ -10047,7 +10057,7 @@
         <v>67</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>54</v>
@@ -10202,7 +10212,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="F17">
         <v>0.91</v>
@@ -10210,7 +10220,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -10218,7 +10228,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -10226,7 +10236,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -10234,7 +10244,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -10242,7 +10252,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -10250,7 +10260,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -10258,7 +10268,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -10266,7 +10276,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -10274,7 +10284,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26">
         <v>0.82</v>
@@ -10282,7 +10292,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -10290,7 +10300,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -10298,7 +10308,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -10306,7 +10316,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -10314,7 +10324,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -28230,7 +28240,7 @@
   <dimension ref="A1:H313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E275" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J304" sqref="J304"/>
@@ -35704,9 +35714,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -35722,7 +35739,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -36681,7 +36698,7 @@
         <v>53</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66">
@@ -36697,9 +36714,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -36715,10 +36739,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -36726,7 +36750,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
@@ -36744,7 +36768,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
@@ -36762,7 +36786,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
@@ -36780,7 +36804,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
@@ -36798,7 +36822,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -36816,7 +36840,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
@@ -36834,7 +36858,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
@@ -36852,7 +36876,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
@@ -36870,7 +36894,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -36888,7 +36912,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
@@ -36906,7 +36930,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
@@ -36924,7 +36948,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
@@ -36942,7 +36966,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
@@ -36960,7 +36984,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
@@ -36978,7 +37002,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
@@ -36996,7 +37020,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -37014,7 +37038,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
@@ -37032,7 +37056,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
@@ -37050,7 +37074,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -37068,7 +37092,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -37086,7 +37110,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2">
@@ -37104,7 +37128,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2">
@@ -37122,7 +37146,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2">
@@ -37140,7 +37164,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2">
@@ -37158,7 +37182,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2">
@@ -37176,7 +37200,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
@@ -37194,7 +37218,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
@@ -37212,7 +37236,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2">
@@ -37230,7 +37254,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2">
@@ -37248,7 +37272,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2">
@@ -37266,7 +37290,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -37301,7 +37325,7 @@
         <v>45</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34">
@@ -37350,28 +37374,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -38488,7 +38512,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -38652,7 +38676,7 @@
         <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>54</v>
@@ -39140,7 +39164,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2">
@@ -39155,7 +39179,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2">
@@ -39170,7 +39194,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2">
@@ -39185,7 +39209,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2">
@@ -39200,7 +39224,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2">
@@ -39215,7 +39239,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2">
@@ -39230,7 +39254,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
@@ -39245,7 +39269,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2">
@@ -39260,7 +39284,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
@@ -39275,7 +39299,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -39290,7 +39314,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
@@ -39305,7 +39329,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
@@ -39320,7 +39344,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -39335,7 +39359,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
@@ -39350,7 +39374,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
@@ -39365,7 +39389,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -39380,7 +39404,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -39395,7 +39419,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
@@ -39410,7 +39434,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -39425,7 +39449,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -39440,7 +39464,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -39455,7 +39479,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
@@ -39470,7 +39494,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
@@ -39485,7 +39509,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2">
@@ -39500,7 +39524,7 @@
         <v>8</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
@@ -39515,7 +39539,7 @@
         <v>8</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2">
@@ -39530,7 +39554,7 @@
         <v>8</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2">
@@ -39545,7 +39569,7 @@
         <v>8</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2">
@@ -39560,7 +39584,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2">
@@ -39575,7 +39599,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2">
@@ -39590,7 +39614,7 @@
         <v>8</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2">
@@ -39647,7 +39671,7 @@
         <v>8</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2">
@@ -39704,7 +39728,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2">
@@ -39761,7 +39785,7 @@
         <v>8</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2">
@@ -39818,7 +39842,7 @@
         <v>8</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2">
@@ -39875,7 +39899,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2">
@@ -39932,7 +39956,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2">
@@ -39989,7 +40013,7 @@
         <v>8</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2">
@@ -40046,7 +40070,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
@@ -40103,7 +40127,7 @@
         <v>8</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2">
@@ -40160,7 +40184,7 @@
         <v>8</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2">
@@ -40217,7 +40241,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2">
@@ -40274,7 +40298,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2">
@@ -40331,7 +40355,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2">
@@ -40388,7 +40412,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2">
@@ -40445,7 +40469,7 @@
         <v>8</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2">
@@ -40502,7 +40526,7 @@
         <v>8</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2">
@@ -40559,7 +40583,7 @@
         <v>8</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2">
@@ -40616,7 +40640,7 @@
         <v>8</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2">
@@ -40673,7 +40697,7 @@
         <v>8</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2">
@@ -40730,7 +40754,7 @@
         <v>8</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2">
@@ -40787,7 +40811,7 @@
         <v>8</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2">
@@ -40844,7 +40868,7 @@
         <v>8</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2">
@@ -40901,7 +40925,7 @@
         <v>8</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2">
@@ -40958,7 +40982,7 @@
         <v>8</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2">
@@ -41015,7 +41039,7 @@
         <v>8</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2">
@@ -41072,7 +41096,7 @@
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2">
@@ -41129,7 +41153,7 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2">
@@ -41186,7 +41210,7 @@
         <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2">
@@ -41243,7 +41267,7 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2">
@@ -41300,7 +41324,7 @@
         <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2">
@@ -41315,7 +41339,7 @@
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2">
@@ -41330,7 +41354,7 @@
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2">
@@ -41345,7 +41369,7 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2">
@@ -41360,7 +41384,7 @@
         <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2">
@@ -41375,7 +41399,7 @@
         <v>8</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2">
@@ -41390,7 +41414,7 @@
         <v>8</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2">
@@ -41405,7 +41429,7 @@
         <v>8</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2">
@@ -41420,7 +41444,7 @@
         <v>8</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2">
@@ -41435,7 +41459,7 @@
         <v>8</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2">
@@ -41450,7 +41474,7 @@
         <v>8</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2">
@@ -41465,7 +41489,7 @@
         <v>8</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2">
@@ -41480,7 +41504,7 @@
         <v>8</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2">
@@ -41495,7 +41519,7 @@
         <v>8</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2">
@@ -41510,7 +41534,7 @@
         <v>8</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2">
@@ -41525,7 +41549,7 @@
         <v>8</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2">
@@ -41540,7 +41564,7 @@
         <v>8</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2">
@@ -41555,7 +41579,7 @@
         <v>8</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2">
@@ -41570,7 +41594,7 @@
         <v>8</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2">
@@ -41585,7 +41609,7 @@
         <v>8</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2">
@@ -41600,7 +41624,7 @@
         <v>8</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2">
@@ -41615,7 +41639,7 @@
         <v>8</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2">
@@ -41630,7 +41654,7 @@
         <v>8</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2">
@@ -41645,7 +41669,7 @@
         <v>8</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2">
@@ -41660,7 +41684,7 @@
         <v>8</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2">
@@ -41675,7 +41699,7 @@
         <v>8</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2">
@@ -41690,7 +41714,7 @@
         <v>8</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2">
@@ -41705,7 +41729,7 @@
         <v>8</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2">
@@ -41720,7 +41744,7 @@
         <v>8</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2">
@@ -41735,7 +41759,7 @@
         <v>8</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2">
@@ -41750,7 +41774,7 @@
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2">
@@ -41765,7 +41789,7 @@
         <v>8</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2">
@@ -41780,7 +41804,7 @@
         <v>8</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="2">
@@ -41795,7 +41819,7 @@
         <v>8</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2">
@@ -41810,7 +41834,7 @@
         <v>8</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2">
@@ -41825,7 +41849,7 @@
         <v>8</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2">
@@ -41840,7 +41864,7 @@
         <v>8</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" s="2">
@@ -41855,7 +41879,7 @@
         <v>8</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2">
@@ -41870,7 +41894,7 @@
         <v>8</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="2">
@@ -41885,7 +41909,7 @@
         <v>8</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="2">
@@ -41900,7 +41924,7 @@
         <v>8</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2">
@@ -41915,7 +41939,7 @@
         <v>8</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="2">
@@ -41930,7 +41954,7 @@
         <v>8</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2">
@@ -41945,7 +41969,7 @@
         <v>8</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="2">
@@ -41960,7 +41984,7 @@
         <v>8</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="2">
@@ -41975,7 +41999,7 @@
         <v>8</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="2">
@@ -41990,7 +42014,7 @@
         <v>8</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="2">
@@ -42005,7 +42029,7 @@
         <v>8</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C139" s="2"/>
       <c r="D139" s="2">
@@ -42020,7 +42044,7 @@
         <v>8</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2">
@@ -42035,7 +42059,7 @@
         <v>8</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="2">
@@ -42050,7 +42074,7 @@
         <v>8</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2">
@@ -42065,7 +42089,7 @@
         <v>8</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" s="2">
@@ -42080,7 +42104,7 @@
         <v>8</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2">
@@ -42095,7 +42119,7 @@
         <v>8</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2">
@@ -42110,7 +42134,7 @@
         <v>8</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2">
@@ -42125,7 +42149,7 @@
         <v>8</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C147" s="2"/>
       <c r="D147" s="2">
@@ -42140,7 +42164,7 @@
         <v>8</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="2">
@@ -42155,7 +42179,7 @@
         <v>8</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="2">
@@ -42170,7 +42194,7 @@
         <v>8</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="2">
@@ -42185,7 +42209,7 @@
         <v>8</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="2">
@@ -42200,7 +42224,7 @@
         <v>33</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -42213,7 +42237,7 @@
         <v>33</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -42226,7 +42250,7 @@
         <v>5</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
@@ -42246,6 +42270,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -42261,7 +42288,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Transport: PHEV and Trains.
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v3.xlsx
+++ b/data/cnf_files/restore_cnf_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC4B793-5F58-6545-8CA0-D090A18E51CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD660962-5E6D-C54F-B8D7-A0C7A1F4A790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="36700" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="36700" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,17 @@
     <sheet name="FiE" sheetId="11" r:id="rId11"/>
     <sheet name="FoE" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -434,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -442,6 +452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3862,8 +3873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="B315" sqref="B315"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="H152" sqref="H152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10034,7 +10045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -28239,11 +28250,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H313"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J304" sqref="J304"/>
+      <selection pane="bottomRight" activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31895,7 +31906,7 @@
         <v>1990</v>
       </c>
       <c r="E152">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F152">
         <v>25173.572774112639</v>
@@ -31919,7 +31930,7 @@
         <v>1991</v>
       </c>
       <c r="E153">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F153">
         <v>25173.572774112639</v>
@@ -31943,7 +31954,7 @@
         <v>1992</v>
       </c>
       <c r="E154">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F154">
         <v>25173.572774112639</v>
@@ -31967,7 +31978,7 @@
         <v>1993</v>
       </c>
       <c r="E155">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F155">
         <v>25173.572774112639</v>
@@ -31991,7 +32002,7 @@
         <v>1994</v>
       </c>
       <c r="E156">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F156">
         <v>25173.572774112639</v>
@@ -32015,7 +32026,7 @@
         <v>1995</v>
       </c>
       <c r="E157">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F157">
         <v>25173.572774112639</v>
@@ -32039,7 +32050,7 @@
         <v>1996</v>
       </c>
       <c r="E158">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F158">
         <v>25173.572774112639</v>
@@ -32063,7 +32074,7 @@
         <v>1997</v>
       </c>
       <c r="E159">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F159">
         <v>25173.572774112639</v>
@@ -32087,7 +32098,7 @@
         <v>1998</v>
       </c>
       <c r="E160">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F160">
         <v>25173.572774112639</v>
@@ -32111,7 +32122,7 @@
         <v>1999</v>
       </c>
       <c r="E161">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F161">
         <v>25173.572774112639</v>
@@ -32135,7 +32146,7 @@
         <v>2000</v>
       </c>
       <c r="E162">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F162">
         <v>25173.572774112639</v>
@@ -32159,7 +32170,7 @@
         <v>2001</v>
       </c>
       <c r="E163">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F163">
         <v>25173.572774112639</v>
@@ -32183,7 +32194,7 @@
         <v>2002</v>
       </c>
       <c r="E164">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F164">
         <v>25173.572774112639</v>
@@ -32207,7 +32218,7 @@
         <v>2003</v>
       </c>
       <c r="E165">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F165">
         <v>25173.572774112639</v>
@@ -32231,7 +32242,7 @@
         <v>2004</v>
       </c>
       <c r="E166">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F166">
         <v>25173.572774112639</v>
@@ -32255,7 +32266,7 @@
         <v>2005</v>
       </c>
       <c r="E167">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F167">
         <v>25173.572774112639</v>
@@ -32279,7 +32290,7 @@
         <v>2006</v>
       </c>
       <c r="E168">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F168">
         <v>25173.572774112639</v>
@@ -32303,7 +32314,7 @@
         <v>2007</v>
       </c>
       <c r="E169">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F169">
         <v>25173.572774112639</v>
@@ -32327,7 +32338,7 @@
         <v>2008</v>
       </c>
       <c r="E170">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F170">
         <v>25173.572774112639</v>
@@ -32351,7 +32362,7 @@
         <v>2009</v>
       </c>
       <c r="E171">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F171">
         <v>25173.572774112639</v>
@@ -32375,7 +32386,7 @@
         <v>2010</v>
       </c>
       <c r="E172">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F172">
         <v>25173.572774112639</v>
@@ -32399,7 +32410,7 @@
         <v>2011</v>
       </c>
       <c r="E173">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F173">
         <v>25173.572774112639</v>
@@ -32423,7 +32434,7 @@
         <v>2012</v>
       </c>
       <c r="E174">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F174">
         <v>25173.572774112639</v>
@@ -32447,7 +32458,7 @@
         <v>2013</v>
       </c>
       <c r="E175">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F175">
         <v>25173.572774112639</v>
@@ -32471,7 +32482,7 @@
         <v>2014</v>
       </c>
       <c r="E176">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F176">
         <v>25173.572774112639</v>
@@ -32495,7 +32506,7 @@
         <v>2015</v>
       </c>
       <c r="E177">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F177">
         <v>25173.572774112639</v>
@@ -32519,7 +32530,7 @@
         <v>2016</v>
       </c>
       <c r="E178">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F178">
         <v>25173.572774112639</v>
@@ -32543,7 +32554,7 @@
         <v>2017</v>
       </c>
       <c r="E179">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F179">
         <v>25173.572774112639</v>
@@ -32567,7 +32578,7 @@
         <v>2018</v>
       </c>
       <c r="E180">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F180">
         <v>25173.572774112639</v>
@@ -32591,7 +32602,7 @@
         <v>2019</v>
       </c>
       <c r="E181">
-        <v>26212.949088670612</v>
+        <v>24000</v>
       </c>
       <c r="F181">
         <v>25173.572774112639</v>
@@ -35539,8 +35550,8 @@
       <c r="E304">
         <v>1.4710886986301371E-6</v>
       </c>
-      <c r="F304">
-        <v>1.4710886986301371E-6</v>
+      <c r="F304" s="3">
+        <v>1.4710886986301401E-6</v>
       </c>
       <c r="G304">
         <v>1.4710886986301371E-6</v>
@@ -36715,7 +36726,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36723,6 +36734,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -36760,7 +36772,7 @@
         <v>46.578000000000003</v>
       </c>
       <c r="F2">
-        <v>37182.671856110719</v>
+        <v>44619.206227332863</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -36778,7 +36790,7 @@
         <v>47.585999999999999</v>
       </c>
       <c r="F3">
-        <v>38134.297164335228</v>
+        <v>45761.156597202273</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -36796,7 +36808,7 @@
         <v>47.866</v>
       </c>
       <c r="F4">
-        <v>37638.17477853255</v>
+        <v>45165.809734239061</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -36814,7 +36826,7 @@
         <v>47.238999999999997</v>
       </c>
       <c r="F5">
-        <v>36835.518338482259</v>
+        <v>44202.62200617871</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -36832,7 +36844,7 @@
         <v>46.896999999999998</v>
       </c>
       <c r="F6">
-        <v>35683.674102653596</v>
+        <v>42820.408923184317</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -36850,7 +36862,7 @@
         <v>47.881999999999998</v>
       </c>
       <c r="F7">
-        <v>36018.509246463604</v>
+        <v>43222.21109575632</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -36868,7 +36880,7 @@
         <v>48.692</v>
       </c>
       <c r="F8">
-        <v>36331.283792763723</v>
+        <v>43597.540551316466</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -36886,7 +36898,7 @@
         <v>48.612000000000002</v>
       </c>
       <c r="F9">
-        <v>36999.729664132923</v>
+        <v>44399.675596959503</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -36904,7 +36916,7 @@
         <v>49.62</v>
       </c>
       <c r="F10">
-        <v>37868.30045079931</v>
+        <v>45441.960540959168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -36922,7 +36934,7 @@
         <v>51.213000000000001</v>
       </c>
       <c r="F11">
-        <v>38708.67147562997</v>
+        <v>46450.405770755962</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -36940,7 +36952,7 @@
         <v>52.372999999999998</v>
       </c>
       <c r="F12">
-        <v>39761.205073119178</v>
+        <v>47713.44608774301</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -36958,7 +36970,7 @@
         <v>53.749000000000002</v>
       </c>
       <c r="F13">
-        <v>40274.809679596263</v>
+        <v>48329.771615515514</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -36976,7 +36988,7 @@
         <v>54.029000000000003</v>
       </c>
       <c r="F14">
-        <v>40829.883259365437</v>
+        <v>48995.85991123852</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -36994,7 +37006,7 @@
         <v>55.122</v>
       </c>
       <c r="F15">
-        <v>41251.379860000103</v>
+        <v>49501.65583200012</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -37012,7 +37024,7 @@
         <v>56.170999999999999</v>
       </c>
       <c r="F16">
-        <v>41712.729229201497</v>
+        <v>50055.275075041798</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -37030,7 +37042,7 @@
         <v>57.33</v>
       </c>
       <c r="F17">
-        <v>41870.466032408287</v>
+        <v>50244.559238889946</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -37048,7 +37060,7 @@
         <v>57.781999999999996</v>
       </c>
       <c r="F18">
-        <v>42115.666519103441</v>
+        <v>50538.799822924128</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -37066,7 +37078,7 @@
         <v>57.432000000000002</v>
       </c>
       <c r="F19">
-        <v>42445.951857959852</v>
+        <v>50935.14222955182</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -37084,7 +37096,7 @@
         <v>58.728999999999999</v>
       </c>
       <c r="F20">
-        <v>43394.771519945287</v>
+        <v>52073.725823934343</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -37102,7 +37114,7 @@
         <v>57.494</v>
       </c>
       <c r="F21">
-        <v>44496.552849528918</v>
+        <v>53395.863419434703</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -37120,7 +37132,7 @@
         <v>59.784999999999997</v>
       </c>
       <c r="F22">
-        <v>45318.975799582127</v>
+        <v>54382.77095949855</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -37138,7 +37150,7 @@
         <v>58.598999999999997</v>
       </c>
       <c r="F23">
-        <v>45858.129594139318</v>
+        <v>55029.755512967182</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -37156,7 +37168,7 @@
         <v>58.972999999999999</v>
       </c>
       <c r="F24">
-        <v>46738.892681957972</v>
+        <v>56086.671218349562</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -37174,7 +37186,7 @@
         <v>59.323</v>
       </c>
       <c r="F25">
-        <v>47566.930495956032</v>
+        <v>57080.31659514724</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -37192,7 +37204,7 @@
         <v>57.466000000000001</v>
       </c>
       <c r="F26">
-        <v>48358.321346343153</v>
+        <v>58029.985615611782</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -37210,7 +37222,7 @@
         <v>58.246000000000002</v>
       </c>
       <c r="F27">
-        <v>49153.01937952076</v>
+        <v>58983.623255424907</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -37228,7 +37240,7 @@
         <v>58.238999999999997</v>
       </c>
       <c r="F28">
-        <v>50058.343063967557</v>
+        <v>60070.011676761067</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -37246,7 +37258,7 @@
         <v>58.482999999999997</v>
       </c>
       <c r="F29">
-        <v>50848.81811713428</v>
+        <v>61018.581740561131</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -37264,7 +37276,7 @@
         <v>57.646999999999998</v>
       </c>
       <c r="F30">
-        <v>51281.32206503769</v>
+        <v>61537.586478045225</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -37282,7 +37294,7 @@
         <v>57.198</v>
       </c>
       <c r="F31">
-        <v>51558.537232099763</v>
+        <v>61870.24467851971</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>